<commit_message>
Modif intelligence et ajout BOM
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projet\Compagnie\GitKraken\Mr.DriveShaft\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E5827E-B3BF-42FB-A338-8FCF72C10D15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E557907-AC46-4A07-80A4-B1865E164038}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="225" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="118">
   <si>
     <t>BOM : Mr.DriveShaft</t>
   </si>
@@ -345,6 +345,48 @@
   </si>
   <si>
     <t>Prix 4ACC : 208,20</t>
+  </si>
+  <si>
+    <t>Maison</t>
+  </si>
+  <si>
+    <t>Taxe</t>
+  </si>
+  <si>
+    <t>Total avec taxe</t>
+  </si>
+  <si>
+    <t>Total par commancede</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total sur facture </t>
+  </si>
+  <si>
+    <t>digikey</t>
+  </si>
+  <si>
+    <t>Commande</t>
+  </si>
+  <si>
+    <t># de facture WEB</t>
+  </si>
+  <si>
+    <t>PAYPAL</t>
+  </si>
+  <si>
+    <t>: 7D6288831N3459918 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amazon </t>
+  </si>
+  <si>
+    <t>702-2278557-4097849</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total </t>
   </si>
 </sst>
 </file>
@@ -407,28 +449,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
     <cellStyle name="Monétaire" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Pourcentage" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -767,10 +812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R30"/>
+  <dimension ref="A1:T43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,21 +827,23 @@
     <col min="5" max="5" width="3.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26.5703125" customWidth="1"/>
     <col min="10" max="10" width="19.28515625" customWidth="1"/>
     <col min="11" max="11" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="98.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.42578125" customWidth="1"/>
     <col min="14" max="14" width="10" customWidth="1"/>
     <col min="15" max="17" width="13" customWidth="1"/>
     <col min="18" max="18" width="11" customWidth="1"/>
+    <col min="20" max="20" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2"/>
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -813,9 +860,9 @@
       <c r="B3" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <f>SUM(Tableau1[Total $$$])</f>
-        <v>214.94</v>
+        <v>230.73000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -899,28 +946,28 @@
       <c r="K6" t="s">
         <v>26</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L6" s="2" t="s">
         <v>27</v>
       </c>
       <c r="M6">
         <v>1</v>
       </c>
       <c r="N6">
-        <v>4</v>
-      </c>
-      <c r="O6" s="4">
+        <v>5</v>
+      </c>
+      <c r="O6" s="3">
         <v>13.27</v>
       </c>
-      <c r="P6" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="4">
+      <c r="P6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="3">
         <f>Tableau1[[#This Row],[price/bag $]]/Tableau1[[#This Row],[nb/bag]]</f>
         <v>13.27</v>
       </c>
-      <c r="R6" s="4">
+      <c r="R6" s="3">
         <f>Tableau1[[#This Row],[price/bag $]]*Tableau1[[#This Row],[Qty buy]]+Tableau1[[#This Row],[Shpping $]]</f>
-        <v>53.08</v>
+        <v>66.349999999999994</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -954,7 +1001,7 @@
       <c r="K7" t="s">
         <v>32</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="L7" s="2" t="s">
         <v>33</v>
       </c>
       <c r="M7">
@@ -963,17 +1010,17 @@
       <c r="N7">
         <v>2</v>
       </c>
-      <c r="O7" s="4">
+      <c r="O7" s="3">
         <v>4.5</v>
       </c>
-      <c r="P7" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="4">
+      <c r="P7" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="3">
         <f>Tableau1[[#This Row],[price/bag $]]/Tableau1[[#This Row],[nb/bag]]</f>
         <v>4.5</v>
       </c>
-      <c r="R7" s="4">
+      <c r="R7" s="3">
         <f>Tableau1[[#This Row],[price/bag $]]*Tableau1[[#This Row],[Qty buy]]+Tableau1[[#This Row],[Shpping $]]</f>
         <v>9</v>
       </c>
@@ -1000,7 +1047,7 @@
       <c r="J8" t="s">
         <v>96</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="2" t="s">
         <v>97</v>
       </c>
       <c r="M8">
@@ -1009,17 +1056,17 @@
       <c r="N8">
         <v>1</v>
       </c>
-      <c r="O8" s="4">
+      <c r="O8" s="3">
         <v>5.44</v>
       </c>
-      <c r="P8" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="4">
+      <c r="P8" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="3">
         <f>Tableau1[[#This Row],[price/bag $]]/Tableau1[[#This Row],[nb/bag]]</f>
         <v>0.54400000000000004</v>
       </c>
-      <c r="R8" s="4">
+      <c r="R8" s="3">
         <f>Tableau1[[#This Row],[price/bag $]]*Tableau1[[#This Row],[Qty buy]]+Tableau1[[#This Row],[Shpping $]]</f>
         <v>5.44</v>
       </c>
@@ -1037,15 +1084,15 @@
       <c r="D9">
         <v>1</v>
       </c>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="4" t="e">
+      <c r="O9" s="3"/>
+      <c r="P9" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="3" t="e">
         <f>Tableau1[[#This Row],[price/bag $]]/Tableau1[[#This Row],[nb/bag]]</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="R9" s="4">
+      <c r="R9" s="3">
         <f>Tableau1[[#This Row],[price/bag $]]*Tableau1[[#This Row],[Qty buy]]+Tableau1[[#This Row],[Shpping $]]</f>
         <v>0</v>
       </c>
@@ -1078,17 +1125,17 @@
       <c r="N10">
         <v>1</v>
       </c>
-      <c r="O10" s="4">
+      <c r="O10" s="3">
         <v>20</v>
       </c>
-      <c r="P10" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="4">
+      <c r="P10" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="3">
         <f>Tableau1[[#This Row],[price/bag $]]/Tableau1[[#This Row],[nb/bag]]</f>
         <v>20</v>
       </c>
-      <c r="R10" s="4">
+      <c r="R10" s="3">
         <f>Tableau1[[#This Row],[price/bag $]]*Tableau1[[#This Row],[Qty buy]]+Tableau1[[#This Row],[Shpping $]]</f>
         <v>20</v>
       </c>
@@ -1124,7 +1171,7 @@
       <c r="K11" t="s">
         <v>68</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="L11" s="2" t="s">
         <v>69</v>
       </c>
       <c r="M11">
@@ -1133,17 +1180,17 @@
       <c r="N11">
         <v>2</v>
       </c>
-      <c r="O11" s="4">
+      <c r="O11" s="3">
         <v>2.2400000000000002</v>
       </c>
-      <c r="P11" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="4">
+      <c r="P11" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="3">
         <f>Tableau1[[#This Row],[price/bag $]]/Tableau1[[#This Row],[nb/bag]]</f>
         <v>2.2400000000000002</v>
       </c>
-      <c r="R11" s="4">
+      <c r="R11" s="3">
         <f>Tableau1[[#This Row],[price/bag $]]*Tableau1[[#This Row],[Qty buy]]+Tableau1[[#This Row],[Shpping $]]</f>
         <v>4.4800000000000004</v>
       </c>
@@ -1161,15 +1208,18 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="4" t="e">
+      <c r="H12" t="s">
+        <v>104</v>
+      </c>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="3" t="e">
         <f>Tableau1[[#This Row],[price/bag $]]/Tableau1[[#This Row],[nb/bag]]</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="R12" s="4">
+      <c r="R12" s="3">
         <f>Tableau1[[#This Row],[price/bag $]]*Tableau1[[#This Row],[Qty buy]]+Tableau1[[#This Row],[Shpping $]]</f>
         <v>0</v>
       </c>
@@ -1205,28 +1255,28 @@
       <c r="K13" t="s">
         <v>64</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="L13" s="2" t="s">
         <v>60</v>
       </c>
       <c r="M13">
         <v>1</v>
       </c>
       <c r="N13">
-        <v>1</v>
-      </c>
-      <c r="O13" s="4">
+        <v>2</v>
+      </c>
+      <c r="O13" s="3">
         <v>2.52</v>
       </c>
-      <c r="P13" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="4">
+      <c r="P13" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="3">
         <f>Tableau1[[#This Row],[price/bag $]]/Tableau1[[#This Row],[nb/bag]]</f>
         <v>2.52</v>
       </c>
-      <c r="R13" s="4">
+      <c r="R13" s="3">
         <f>Tableau1[[#This Row],[price/bag $]]*Tableau1[[#This Row],[Qty buy]]+Tableau1[[#This Row],[Shpping $]]</f>
-        <v>2.52</v>
+        <v>5.04</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -1260,7 +1310,7 @@
       <c r="K14" t="s">
         <v>58</v>
       </c>
-      <c r="L14" s="3" t="s">
+      <c r="L14" s="2" t="s">
         <v>59</v>
       </c>
       <c r="M14">
@@ -1269,17 +1319,17 @@
       <c r="N14">
         <v>1</v>
       </c>
-      <c r="O14" s="4">
+      <c r="O14" s="3">
         <v>49.17</v>
       </c>
-      <c r="P14" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="4">
+      <c r="P14" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="3">
         <f>Tableau1[[#This Row],[price/bag $]]/Tableau1[[#This Row],[nb/bag]]</f>
         <v>49.17</v>
       </c>
-      <c r="R14" s="4">
+      <c r="R14" s="3">
         <f>Tableau1[[#This Row],[price/bag $]]*Tableau1[[#This Row],[Qty buy]]+Tableau1[[#This Row],[Shpping $]]</f>
         <v>49.17</v>
       </c>
@@ -1315,7 +1365,7 @@
       <c r="K15" t="s">
         <v>81</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="L15" s="2" t="s">
         <v>78</v>
       </c>
       <c r="M15">
@@ -1324,17 +1374,17 @@
       <c r="N15">
         <v>5</v>
       </c>
-      <c r="O15" s="4">
+      <c r="O15" s="3">
         <v>8.69</v>
       </c>
-      <c r="P15" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="4">
+      <c r="P15" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="3">
         <f>Tableau1[[#This Row],[price/bag $]]/Tableau1[[#This Row],[nb/bag]]</f>
         <v>8.69</v>
       </c>
-      <c r="R15" s="4">
+      <c r="R15" s="3">
         <f>Tableau1[[#This Row],[price/bag $]]*Tableau1[[#This Row],[Qty buy]]+Tableau1[[#This Row],[Shpping $]]</f>
         <v>43.449999999999996</v>
       </c>
@@ -1361,7 +1411,7 @@
       <c r="J16" t="s">
         <v>100</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="L16" s="2" t="s">
         <v>98</v>
       </c>
       <c r="M16">
@@ -1370,22 +1420,22 @@
       <c r="N16">
         <v>1</v>
       </c>
-      <c r="O16" s="4">
+      <c r="O16" s="3">
         <v>7.93</v>
       </c>
-      <c r="P16" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="4">
+      <c r="P16" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="3">
         <f>Tableau1[[#This Row],[price/bag $]]/Tableau1[[#This Row],[nb/bag]]</f>
         <v>7.93</v>
       </c>
-      <c r="R16" s="4">
+      <c r="R16" s="3">
         <f>Tableau1[[#This Row],[price/bag $]]*Tableau1[[#This Row],[Qty buy]]+Tableau1[[#This Row],[Shpping $]]</f>
         <v>7.93</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>12</v>
       </c>
@@ -1398,20 +1448,20 @@
       <c r="D17">
         <v>2</v>
       </c>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="4" t="e">
+      <c r="O17" s="3"/>
+      <c r="P17" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="3" t="e">
         <f>Tableau1[[#This Row],[price/bag $]]/Tableau1[[#This Row],[nb/bag]]</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="R17" s="4">
+      <c r="R17" s="3">
         <f>Tableau1[[#This Row],[price/bag $]]*Tableau1[[#This Row],[Qty buy]]+Tableau1[[#This Row],[Shpping $]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>13</v>
       </c>
@@ -1424,20 +1474,20 @@
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="4" t="e">
+      <c r="O18" s="3"/>
+      <c r="P18" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="3" t="e">
         <f>Tableau1[[#This Row],[price/bag $]]/Tableau1[[#This Row],[nb/bag]]</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="R18" s="4">
+      <c r="R18" s="3">
         <f>Tableau1[[#This Row],[price/bag $]]*Tableau1[[#This Row],[Qty buy]]+Tableau1[[#This Row],[Shpping $]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>14</v>
       </c>
@@ -1450,74 +1500,74 @@
       <c r="D19">
         <v>1</v>
       </c>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="4" t="e">
+      <c r="O19" s="3"/>
+      <c r="P19" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="3" t="e">
         <f>Tableau1[[#This Row],[price/bag $]]/Tableau1[[#This Row],[nb/bag]]</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="R19" s="4">
+      <c r="R19" s="3">
         <f>Tableau1[[#This Row],[price/bag $]]*Tableau1[[#This Row],[Qty buy]]+Tableau1[[#This Row],[Shpping $]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>15</v>
       </c>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="4" t="e">
+      <c r="O20" s="3"/>
+      <c r="P20" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="3" t="e">
         <f>Tableau1[[#This Row],[price/bag $]]/Tableau1[[#This Row],[nb/bag]]</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="R20" s="4">
+      <c r="R20" s="3">
         <f>Tableau1[[#This Row],[price/bag $]]*Tableau1[[#This Row],[Qty buy]]+Tableau1[[#This Row],[Shpping $]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>16</v>
       </c>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="4" t="e">
+      <c r="O21" s="3"/>
+      <c r="P21" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="3" t="e">
         <f>Tableau1[[#This Row],[price/bag $]]/Tableau1[[#This Row],[nb/bag]]</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="R21" s="4">
+      <c r="R21" s="3">
         <f>Tableau1[[#This Row],[price/bag $]]*Tableau1[[#This Row],[Qty buy]]+Tableau1[[#This Row],[Shpping $]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>17</v>
       </c>
       <c r="B22" t="s">
         <v>70</v>
       </c>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="4" t="e">
+      <c r="O22" s="3"/>
+      <c r="P22" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="3" t="e">
         <f>Tableau1[[#This Row],[price/bag $]]/Tableau1[[#This Row],[nb/bag]]</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="R22" s="4">
+      <c r="R22" s="3">
         <f>Tableau1[[#This Row],[price/bag $]]*Tableau1[[#This Row],[Qty buy]]+Tableau1[[#This Row],[Shpping $]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>18</v>
       </c>
@@ -1539,7 +1589,7 @@
       <c r="J23" t="s">
         <v>74</v>
       </c>
-      <c r="L23" s="3" t="s">
+      <c r="L23" s="2" t="s">
         <v>73</v>
       </c>
       <c r="M23">
@@ -1548,63 +1598,64 @@
       <c r="N23">
         <v>10</v>
       </c>
-      <c r="O23" s="4">
+      <c r="O23" s="3">
         <v>0.38400000000000001</v>
       </c>
-      <c r="P23" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="4">
+      <c r="P23" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="3">
         <f>Tableau1[[#This Row],[price/bag $]]/Tableau1[[#This Row],[nb/bag]]</f>
         <v>0.38400000000000001</v>
       </c>
-      <c r="R23" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
+      <c r="R23" s="3">
+        <v>0</v>
+      </c>
+      <c r="T23" s="4"/>
+    </row>
+    <row r="24" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
         <v>19</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="6">
-        <v>1</v>
-      </c>
-      <c r="F24" s="6" t="s">
+      <c r="C24" s="5">
+        <v>1</v>
+      </c>
+      <c r="F24" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="H24" s="6" t="s">
+      <c r="H24" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="K24" s="6" t="s">
+      <c r="K24" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="L24" s="7" t="s">
+      <c r="L24" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="M24" s="6">
+      <c r="M24" s="5">
         <v>5</v>
       </c>
-      <c r="N24" s="6">
-        <v>1</v>
-      </c>
-      <c r="O24" s="8">
+      <c r="N24" s="5">
+        <v>1</v>
+      </c>
+      <c r="O24" s="7">
         <v>13.92</v>
       </c>
-      <c r="P24" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="8">
+      <c r="P24" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="7">
         <f>Tableau1[[#This Row],[price/bag $]]/Tableau1[[#This Row],[nb/bag]]</f>
         <v>2.7839999999999998</v>
       </c>
-      <c r="R24" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R24" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>20</v>
       </c>
@@ -1623,7 +1674,7 @@
       <c r="K25" t="s">
         <v>89</v>
       </c>
-      <c r="L25" s="3" t="s">
+      <c r="L25" s="2" t="s">
         <v>88</v>
       </c>
       <c r="M25">
@@ -1632,56 +1683,153 @@
       <c r="N25">
         <v>1</v>
       </c>
-      <c r="O25" s="4">
+      <c r="O25" s="3">
         <v>19.87</v>
       </c>
-      <c r="P25" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="4">
+      <c r="P25" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="3">
         <f>Tableau1[[#This Row],[price/bag $]]/Tableau1[[#This Row],[nb/bag]]</f>
         <v>19.87</v>
       </c>
-      <c r="R25" s="4">
+      <c r="R25" s="3">
         <f>Tableau1[[#This Row],[price/bag $]]*Tableau1[[#This Row],[Qty buy]]+Tableau1[[#This Row],[Shpping $]]</f>
         <v>19.87</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>21</v>
       </c>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="4" t="e">
+      <c r="O26" s="3"/>
+      <c r="P26" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="3" t="e">
         <f>Tableau1[[#This Row],[price/bag $]]/Tableau1[[#This Row],[nb/bag]]</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="R26" s="4">
+      <c r="R26" s="3">
         <f>Tableau1[[#This Row],[price/bag $]]*Tableau1[[#This Row],[Qty buy]]+Tableau1[[#This Row],[Shpping $]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>23</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>105</v>
+      </c>
+      <c r="I28" s="8">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>24</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>25</v>
+      </c>
+      <c r="H30" t="s">
+        <v>107</v>
+      </c>
+      <c r="I30" t="s">
+        <v>106</v>
+      </c>
+      <c r="J30" t="s">
+        <v>108</v>
+      </c>
+      <c r="K30" t="s">
+        <v>111</v>
+      </c>
+      <c r="L30" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
+        <v>109</v>
+      </c>
+      <c r="H31">
+        <f>SUMIFS(Tableau1[Total $$$],Tableau1[Fournisseur],"Digi-Key")</f>
+        <v>111.13999999999999</v>
+      </c>
+      <c r="I31">
+        <f>H31*(1+I28)</f>
+        <v>127.81099999999998</v>
+      </c>
+      <c r="J31">
+        <v>127.79</v>
+      </c>
+      <c r="K31">
+        <v>63453026</v>
+      </c>
+    </row>
+    <row r="33" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>24</v>
+      </c>
+      <c r="H33">
+        <f>SUMIFS(Tableau1[Total $$$],Tableau1[Fournisseur],"Robotshop")</f>
+        <v>99.59</v>
+      </c>
+      <c r="I33">
+        <f>H33*(1+I28)</f>
+        <v>114.52849999999999</v>
+      </c>
+      <c r="J33">
+        <v>114.5</v>
+      </c>
+      <c r="K33">
+        <v>800019327</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="36" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>114</v>
+      </c>
+      <c r="H36">
+        <v>20</v>
+      </c>
+      <c r="I36">
+        <f>H36*(1+I28)</f>
+        <v>23</v>
+      </c>
+      <c r="J36">
+        <v>23</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="I38" t="s">
+        <v>117</v>
+      </c>
+      <c r="J38">
+        <f>SUM(J31:J36)</f>
+        <v>265.29000000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="H43" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1700,11 +1848,13 @@
     <hyperlink ref="L25" r:id="rId9" xr:uid="{25B9B50E-D605-44FE-B45D-C4A08CA74B8D}"/>
     <hyperlink ref="L8" r:id="rId10" xr:uid="{01BE994F-F9F0-4C22-A975-AD2F51751E7E}"/>
     <hyperlink ref="L16" r:id="rId11" xr:uid="{50DC8123-80B6-40A8-AB65-5B4EDAA70725}"/>
+    <hyperlink ref="L33" r:id="rId12" display="https://eur04.safelinks.protection.outlook.com/?url=https%3A%2F%2Fwww.paypal.com%2Fmyaccount%2Ftransaction%2Fdetails%2F7D6288831N3459918%3Futm_source%3Dunp%26utm_medium%3Demail%26utm_campaign%3DPPX001066%26utm_unptid%3D07c71335-679a-11ea-8a24-b875c0bfd1b3%26ppid%3DPPX001066%26cnac%3DCA%26rsta%3Dfr_CA%26cust%3D7UN759672U957620R%26unptid%3D07c71335-679a-11ea-8a24-b875c0bfd1b3%26calc%3Dbbd883928e733%26unp_tpcid%3Demail-receipt-xclick-payment%26page%3Dmain%3Aemail%3APPX001066%3A%3A%3A%26pgrp%3Dmain%3Aemail%26e%3Dcl%26mchn%3Dem%26s%3Dci%26mail%3Dsys%26xt%3DCtrl_EmailConfirmation_FooterUpdate&amp;data=02%7C01%7C%7Ce6fd6222bdac48152e0808d7c9bdf207%7C84df9e7fe9f640afb435aaaaaaaaaaaa%7C1%7C0%7C637199689948336862&amp;sdata=%2FDTWz0SE%2F9tHrdg20Q56eSUmSbxIc7AXEYBxaxy3HwE%3D&amp;reserved=0" xr:uid="{0866E6BA-FEC1-4026-B10E-88B8CE7C6EA3}"/>
+    <hyperlink ref="K36" r:id="rId13" display="https://nam10.safelinks.protection.outlook.com/?url=https%3A%2F%2Fwww.amazon.ca%2Fgp%2Fr.html%3FC%3D2R083KRCWO7XK%26K%3D2HCLRSRJDXDHL%26M%3Durn%3Artn%3Amsg%3A202003161535291d82c2b7cba247b6982d10c09c00p0na%26R%3D696W6N82BVKR%26T%3DC%26U%3Dhttps%253A%252F%252Fwww.amazon.ca%252Fgp%252Fcss%252Forder-details%253ForderId%253D702-2278557-4097849%2526ref%253DTE_on%2526ref_%253Dpe_3034960_233709270%26H%3D1OWWKAHKOTWAFHRL8FYDEJSKSWWA%26ref_%3Dpe_3034960_233709270&amp;data=02%7C01%7C%7C5d1faeac7e1349276b8408d7c9bfa9ad%7C84df9e7fe9f640afb435aaaaaaaaaaaa%7C1%7C0%7C637199697324461998&amp;sdata=wbsgwtGZ3RSnRtpSHTK3KMRnYLWBfRvSA%2F9rmS7S57c%3D&amp;reserved=0" xr:uid="{61AE96C0-C84A-4E9D-BAC8-98C0F9FA71B6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
   <tableParts count="1">
-    <tablePart r:id="rId13"/>
+    <tablePart r:id="rId15"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>